<commit_message>
Switch from robot to URL + API Key
Co-Authored-By: raymondxyz <79726173+raymondxyz@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/sentiment-analysis/inputData.xlsx
+++ b/sentiment-analysis/inputData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\files.auckland.ac.nz\myhome\Downloads\SentimentAnalysis-20230921T231635Z-001\SentimentAnalysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jia\Documents\git\social-media-analysis\sentiment-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE57D9A2-FCBB-40BF-9E4B-8C6295DC27E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F782DE-B412-4B71-9FD1-5879FF871986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3375" yWindow="3000" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>